<commit_message>
Futher work on Excel add-in.
</commit_message>
<xml_diff>
--- a/samples/excel/storage_samples.xlsx
+++ b/samples/excel/storage_samples.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AC9829-4A3A-47A8-8F41-E12481F6768D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD43B0D-3975-46C8-80A3-82101C6AAE39}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Inject/Withdraw Rates and Costs</t>
-  </si>
-  <si>
     <t>Inventory</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>% Cmdty Used</t>
+  </si>
+  <si>
+    <t>Inject/Withdraw/Inventory Constraints</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
   <dimension ref="B2:N97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +449,7 @@
         <v>43702</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
@@ -457,18 +457,18 @@
         <v>3</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3">
         <v>43678</v>
@@ -479,12 +479,16 @@
       <c r="L5" s="5">
         <v>0</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
+      <c r="M5" s="5">
+        <v>1356</v>
+      </c>
+      <c r="N5" s="5">
+        <v>1525</v>
+      </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3">
         <v>43711</v>
@@ -495,8 +499,12 @@
       <c r="L6" s="5">
         <v>300</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
+      <c r="M6" s="5">
+        <v>1306</v>
+      </c>
+      <c r="N6" s="5">
+        <v>1689</v>
+      </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K7" s="3">
@@ -505,12 +513,16 @@
       <c r="L7" s="5">
         <v>500</v>
       </c>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
+      <c r="M7" s="5">
+        <v>1206</v>
+      </c>
+      <c r="N7" s="5">
+        <v>1711</v>
+      </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K8" s="3">
         <v>43702</v>
@@ -518,12 +530,16 @@
       <c r="L8" s="5">
         <v>600</v>
       </c>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
+      <c r="M8" s="5">
+        <v>1145</v>
+      </c>
+      <c r="N8" s="5">
+        <v>1784</v>
+      </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2">
         <v>0.1</v>
@@ -534,12 +550,16 @@
       <c r="L9" s="5">
         <v>0</v>
       </c>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
+      <c r="M9" s="5">
+        <v>1005</v>
+      </c>
+      <c r="N9" s="5">
+        <v>1587</v>
+      </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="6">
         <v>1E-4</v>
@@ -548,37 +568,49 @@
         <v>43705</v>
       </c>
       <c r="L10" s="5">
-        <v>300</v>
-      </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
+        <v>200</v>
+      </c>
+      <c r="M10" s="5">
+        <v>958</v>
+      </c>
+      <c r="N10" s="5">
+        <v>1604</v>
+      </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K11" s="3">
         <v>43705</v>
       </c>
       <c r="L11" s="5">
-        <v>500</v>
-      </c>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
+        <v>400</v>
+      </c>
+      <c r="M11" s="5">
+        <v>910</v>
+      </c>
+      <c r="N11" s="5">
+        <v>1658</v>
+      </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K12" s="3">
-        <v>43705</v>
+        <v>43709</v>
       </c>
       <c r="L12" s="5">
-        <v>600</v>
-      </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
+        <v>1346</v>
+      </c>
+      <c r="N12" s="5">
+        <v>1479.25</v>
+      </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2">
         <v>0.45</v>
@@ -587,14 +619,18 @@
         <v>43709</v>
       </c>
       <c r="L13" s="5">
-        <v>0</v>
-      </c>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
+        <v>300</v>
+      </c>
+      <c r="M13" s="5">
+        <v>1296</v>
+      </c>
+      <c r="N13" s="5">
+        <v>1638.33</v>
+      </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="6">
         <v>5.0000000000000001E-4</v>
@@ -603,28 +639,32 @@
         <v>43709</v>
       </c>
       <c r="L14" s="5">
-        <v>300</v>
-      </c>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
+        <v>500</v>
+      </c>
+      <c r="M14" s="5">
+        <v>1196</v>
+      </c>
+      <c r="N14" s="5">
+        <v>1659.6699999999998</v>
+      </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K15" s="3">
         <v>43709</v>
       </c>
       <c r="L15" s="5">
-        <v>500</v>
-      </c>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
+        <v>600</v>
+      </c>
+      <c r="M15" s="5">
+        <v>1135</v>
+      </c>
+      <c r="N15" s="5">
+        <v>1730.48</v>
+      </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K16" s="3">
-        <v>43709</v>
-      </c>
-      <c r="L16" s="5">
-        <v>600</v>
-      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
     </row>

</xml_diff>

<commit_message>
Further work on intrinsic valuation Excel function.
</commit_message>
<xml_diff>
--- a/samples/excel/storage_samples.xlsx
+++ b/samples/excel/storage_samples.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD43B0D-3975-46C8-80A3-82101C6AAE39}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046FA925-BEB1-4CA6-A93A-0A02D4DE3B62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="intrinsic_daily" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="CurrentInventory">intrinsic_daily!$C$15</definedName>
     <definedName name="GridSpacing">intrinsic_daily!$C$17</definedName>
-    <definedName name="InjectCmdtyConsumed">intrinsic_daily!$C$10</definedName>
-    <definedName name="InjectCostRate">intrinsic_daily!$C$9</definedName>
-    <definedName name="StorageEnd">intrinsic_daily!$C$6</definedName>
-    <definedName name="StorageStart">intrinsic_daily!$C$5</definedName>
+    <definedName name="InjectCmdtyConsumed">intrinsic_daily!$C$9</definedName>
+    <definedName name="InjectCostRate">intrinsic_daily!$C$8</definedName>
+    <definedName name="StorageEnd">intrinsic_daily!$C$5</definedName>
+    <definedName name="StorageStart">intrinsic_daily!$C$4</definedName>
     <definedName name="ValDate">intrinsic_daily!$C$2</definedName>
-    <definedName name="WithdrawCmdtyConsumed">intrinsic_daily!$C$14</definedName>
-    <definedName name="WithdrawCostRate">intrinsic_daily!$C$13</definedName>
+    <definedName name="WithdrawCmdtyConsumed">intrinsic_daily!$C$13</definedName>
+    <definedName name="WithdrawCostRate">intrinsic_daily!$C$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Valuation Date</t>
   </si>
@@ -81,13 +82,16 @@
   </si>
   <si>
     <t>Inject/Withdraw/Inventory Constraints</t>
+  </si>
+  <si>
+    <t>Current Inventory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,8 +114,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +132,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -133,11 +149,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -145,9 +162,11 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -426,22 +445,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:N97"/>
+  <dimension ref="B1:N97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" customWidth="1"/>
+    <col min="13" max="13" width="15.1796875" customWidth="1"/>
     <col min="14" max="14" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="F1" s="7" t="str">
+        <f>_xll.cmdtyStorageIntrinsicValue(ValDate,StorageStart,StorageEnd,K5:N24,InjectCostRate,InjectCmdtyConsumed,WithdrawCostRate,WithdrawCmdtyConsumed,CurrentInventory,B21:C97,,GridSpacing)</f>
+        <v>Cannot solve for the current period maximum inventory</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,7 +477,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3">
+        <v>43678</v>
+      </c>
       <c r="K4" s="1" t="s">
         <v>3</v>
       </c>
@@ -466,12 +497,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3">
-        <v>43678</v>
+        <v>43711</v>
       </c>
       <c r="K5" s="3">
         <v>43702</v>
@@ -486,13 +517,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3">
-        <v>43711</v>
-      </c>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="K6" s="3">
         <v>43702</v>
       </c>
@@ -506,7 +531,10 @@
         <v>1689</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="K7" s="3">
         <v>43702</v>
       </c>
@@ -520,9 +548,12 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.1</v>
       </c>
       <c r="K8" s="3">
         <v>43702</v>
@@ -537,12 +568,12 @@
         <v>1784</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.1</v>
+        <v>13</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1E-4</v>
       </c>
       <c r="K9" s="3">
         <v>43705</v>
@@ -557,13 +588,7 @@
         <v>1587</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="6">
-        <v>1E-4</v>
-      </c>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
       <c r="K10" s="3">
         <v>43705</v>
       </c>
@@ -577,12 +602,15 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="K11" s="3">
         <v>43705</v>
       </c>
       <c r="L11" s="5">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="M11" s="5">
         <v>910</v>
@@ -591,9 +619,12 @@
         <v>1658</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.45</v>
       </c>
       <c r="K12" s="3">
         <v>43709</v>
@@ -608,12 +639,12 @@
         <v>1479.25</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0.45</v>
+        <v>13</v>
+      </c>
+      <c r="C13" s="6">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K13" s="3">
         <v>43709</v>
@@ -628,13 +659,7 @@
         <v>1638.33</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="6">
-        <v>5.0000000000000001E-4</v>
-      </c>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
       <c r="K14" s="3">
         <v>43709</v>
       </c>
@@ -648,7 +673,13 @@
         <v>1659.6699999999998</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2">
+        <v>500</v>
+      </c>
       <c r="K15" s="3">
         <v>43709</v>
       </c>
@@ -662,13 +693,13 @@
         <v>1730.48</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
       <c r="K16" s="3"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
@@ -680,13 +711,13 @@
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
       <c r="K18" s="3"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
@@ -695,7 +726,7 @@
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
         <v>3</v>
       </c>
@@ -707,7 +738,7 @@
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <v>43702</v>
       </c>
@@ -719,7 +750,7 @@
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B22" s="3">
         <f>B21+1</f>
         <v>43703</v>
@@ -732,7 +763,7 @@
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <f t="shared" ref="B23:B30" si="0">B22+1</f>
         <v>43704</v>
@@ -745,7 +776,7 @@
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>43705</v>
@@ -758,7 +789,7 @@
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>43706</v>
@@ -767,7 +798,7 @@
         <v>50.16228238269035</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>43707</v>
@@ -776,7 +807,7 @@
         <v>50.917998292344571</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>43708</v>
@@ -785,7 +816,7 @@
         <v>50.829710805583225</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>43709</v>
@@ -794,7 +825,7 @@
         <v>49.978591030576084</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>43710</v>
@@ -803,7 +834,7 @@
         <v>49.147154563324776</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>43711</v>
@@ -812,271 +843,271 @@
         <v>49.099820257454425</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B31" s="3"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B32" s="3"/>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" s="3"/>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="3"/>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" s="3"/>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" s="3"/>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" s="3"/>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38" s="3"/>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B39" s="3"/>
       <c r="C39" s="2"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B40" s="3"/>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41" s="3"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42" s="3"/>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B43" s="3"/>
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44" s="3"/>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45" s="3"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46" s="3"/>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47" s="3"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B48" s="3"/>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49" s="3"/>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50" s="3"/>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51" s="3"/>
       <c r="C51" s="2"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52" s="3"/>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53" s="3"/>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54" s="3"/>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55" s="3"/>
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B56" s="3"/>
       <c r="C56" s="2"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" s="3"/>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B58" s="3"/>
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B59" s="3"/>
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B60" s="3"/>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B61" s="3"/>
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B62" s="3"/>
       <c r="C62" s="2"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B63" s="3"/>
       <c r="C63" s="2"/>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B64" s="3"/>
       <c r="C64" s="2"/>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B65" s="3"/>
       <c r="C65" s="2"/>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B66" s="3"/>
       <c r="C66" s="2"/>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B67" s="3"/>
       <c r="C67" s="2"/>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B68" s="3"/>
       <c r="C68" s="2"/>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B69" s="3"/>
       <c r="C69" s="2"/>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B70" s="3"/>
       <c r="C70" s="2"/>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B71" s="3"/>
       <c r="C71" s="2"/>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B72" s="3"/>
       <c r="C72" s="2"/>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B73" s="3"/>
       <c r="C73" s="2"/>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B74" s="3"/>
       <c r="C74" s="2"/>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B75" s="3"/>
       <c r="C75" s="2"/>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B76" s="3"/>
       <c r="C76" s="2"/>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B77" s="3"/>
       <c r="C77" s="2"/>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B78" s="3"/>
       <c r="C78" s="2"/>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B79" s="3"/>
       <c r="C79" s="2"/>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B80" s="3"/>
       <c r="C80" s="2"/>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B81" s="3"/>
       <c r="C81" s="2"/>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B82" s="3"/>
       <c r="C82" s="2"/>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B83" s="3"/>
       <c r="C83" s="2"/>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B84" s="3"/>
       <c r="C84" s="2"/>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B85" s="3"/>
       <c r="C85" s="2"/>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B86" s="3"/>
       <c r="C86" s="2"/>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B87" s="3"/>
       <c r="C87" s="2"/>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B88" s="3"/>
       <c r="C88" s="2"/>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B89" s="3"/>
       <c r="C89" s="2"/>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B90" s="3"/>
       <c r="C90" s="2"/>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B91" s="3"/>
       <c r="C91" s="2"/>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B92" s="3"/>
       <c r="C92" s="2"/>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B93" s="3"/>
       <c r="C93" s="2"/>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B94" s="3"/>
       <c r="C94" s="2"/>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B95" s="3"/>
       <c r="C95" s="2"/>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B96" s="3"/>
       <c r="C96" s="2"/>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B97" s="3"/>
       <c r="C97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Fixed bug in WithTimeAndInventoryVaryingInjectWithdrawRates extension method and added test for bug.
</commit_message>
<xml_diff>
--- a/samples/excel/storage_samples.xlsx
+++ b/samples/excel/storage_samples.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046FA925-BEB1-4CA6-A93A-0A02D4DE3B62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7070C80-CFFF-47C4-8233-C13D517D4069}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -448,7 +448,7 @@
   <dimension ref="B1:N97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -502,7 +502,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="3">
-        <v>43711</v>
+        <v>43710</v>
       </c>
       <c r="K5" s="3">
         <v>43702</v>
@@ -522,7 +522,7 @@
         <v>43702</v>
       </c>
       <c r="L6" s="5">
-        <v>300</v>
+        <v>6000</v>
       </c>
       <c r="M6" s="5">
         <v>1306</v>
@@ -539,7 +539,7 @@
         <v>43702</v>
       </c>
       <c r="L7" s="5">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="M7" s="5">
         <v>1206</v>
@@ -559,7 +559,7 @@
         <v>43702</v>
       </c>
       <c r="L8" s="5">
-        <v>600</v>
+        <v>12000</v>
       </c>
       <c r="M8" s="5">
         <v>1145</v>
@@ -593,7 +593,7 @@
         <v>43705</v>
       </c>
       <c r="L10" s="5">
-        <v>200</v>
+        <v>4000</v>
       </c>
       <c r="M10" s="5">
         <v>958</v>
@@ -610,7 +610,7 @@
         <v>43705</v>
       </c>
       <c r="L11" s="5">
-        <v>600</v>
+        <v>12000</v>
       </c>
       <c r="M11" s="5">
         <v>910</v>
@@ -650,7 +650,7 @@
         <v>43709</v>
       </c>
       <c r="L13" s="5">
-        <v>300</v>
+        <v>6000</v>
       </c>
       <c r="M13" s="5">
         <v>1296</v>
@@ -664,7 +664,7 @@
         <v>43709</v>
       </c>
       <c r="L14" s="5">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="M14" s="5">
         <v>1196</v>
@@ -684,7 +684,7 @@
         <v>43709</v>
       </c>
       <c r="L15" s="5">
-        <v>600</v>
+        <v>12000</v>
       </c>
       <c r="M15" s="5">
         <v>1135</v>

</xml_diff>

<commit_message>
Added Excel function for intrinsic decision profile.
</commit_message>
<xml_diff>
--- a/samples/excel/storage_samples.xlsx
+++ b/samples/excel/storage_samples.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7070C80-CFFF-47C4-8233-C13D517D4069}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D133F8CE-C3A1-4C9D-AE8B-0DD6C7A924A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="intrinsic_daily" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="WithdrawCmdtyConsumed">intrinsic_daily!$C$13</definedName>
     <definedName name="WithdrawCostRate">intrinsic_daily!$C$12</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Valuation Date</t>
   </si>
@@ -86,11 +86,23 @@
   <si>
     <t>Current Inventory</t>
   </si>
+  <si>
+    <t>NPV</t>
+  </si>
+  <si>
+    <t>Decision Profile</t>
+  </si>
+  <si>
+    <t>Inject/Withdraw</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="dd\-mmm\-yy"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -154,7 +166,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -162,7 +174,8 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -448,25 +461,30 @@
   <dimension ref="B1:N97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" customWidth="1"/>
-    <col min="13" max="13" width="15.1796875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
     <col min="14" max="14" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="F1" s="7" t="str">
-        <f>_xll.cmdtyStorageIntrinsicValue(ValDate,StorageStart,StorageEnd,K5:N24,InjectCostRate,InjectCmdtyConsumed,WithdrawCostRate,WithdrawCmdtyConsumed,CurrentInventory,B21:C97,,GridSpacing)</f>
-        <v>Cannot solve for the current period maximum inventory</v>
-      </c>
-    </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="7">
+        <f>_xll.cmdty.StorageIntrinsicValue(ValDate,StorageStart,StorageEnd,K5:N24,InjectCostRate,InjectCmdtyConsumed,WithdrawCostRate,WithdrawCmdtyConsumed,CurrentInventory,B21:C97,,GridSpacing)</f>
+        <v>28160.178279742478</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,13 +495,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3">
         <v>43678</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="K4" s="1" t="s">
         <v>3</v>
       </c>
@@ -497,13 +529,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="3">
         <v>43710</v>
       </c>
+      <c r="E5" s="8">
+        <f t="array" ref="E5:F85">_xll.cmdty.StorageIntrinsicDecisionProfile(ValDate,StorageStart,StorageEnd,K5:N24,InjectCostRate,InjectCmdtyConsumed,WithdrawCostRate,WithdrawCmdtyConsumed,CurrentInventory,B21:C97,,GridSpacing)</f>
+        <v>43702</v>
+      </c>
+      <c r="F5" s="7">
+        <v>-500</v>
+      </c>
+      <c r="G5" s="7">
+        <f>SUM($F$5:F5)+CurrentInventory</f>
+        <v>0</v>
+      </c>
       <c r="K5" s="3">
         <v>43702</v>
       </c>
@@ -517,7 +560,17 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E6" s="8">
+        <v>43703</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1355.9999999999998</v>
+      </c>
+      <c r="G6" s="7">
+        <f>SUM($F$5:F6)+CurrentInventory</f>
+        <v>1355.9999999999998</v>
+      </c>
       <c r="K6" s="3">
         <v>43702</v>
       </c>
@@ -525,16 +578,26 @@
         <v>6000</v>
       </c>
       <c r="M6" s="5">
-        <v>1306</v>
+        <v>1265</v>
       </c>
       <c r="N6" s="5">
         <v>1689</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="E7" s="8">
+        <v>43704</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1323.0752695520002</v>
+      </c>
+      <c r="G7" s="7">
+        <f>SUM($F$5:F7)+CurrentInventory</f>
+        <v>2679.075269552</v>
+      </c>
       <c r="K7" s="3">
         <v>43702</v>
       </c>
@@ -548,13 +611,23 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="2">
         <v>0.1</v>
       </c>
+      <c r="E8" s="8">
+        <v>43705</v>
+      </c>
+      <c r="F8" s="7">
+        <v>973.19242835497414</v>
+      </c>
+      <c r="G8" s="7">
+        <f>SUM($F$5:F8)+CurrentInventory</f>
+        <v>3652.2676979069743</v>
+      </c>
       <c r="K8" s="3">
         <v>43702</v>
       </c>
@@ -568,18 +641,28 @@
         <v>1784</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="6">
         <v>1E-4</v>
       </c>
+      <c r="E9" s="8">
+        <v>43706</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7">
+        <f>SUM($F$5:F9)+CurrentInventory</f>
+        <v>3652.2676979069743</v>
+      </c>
       <c r="K9" s="3">
         <v>43705</v>
       </c>
       <c r="L9" s="5">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="M9" s="5">
         <v>1005</v>
@@ -588,12 +671,22 @@
         <v>1587</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E10" s="8">
+        <v>43707</v>
+      </c>
+      <c r="F10" s="7">
+        <v>-1635.0263865457559</v>
+      </c>
+      <c r="G10" s="7">
+        <f>SUM($F$5:F10)+CurrentInventory</f>
+        <v>2017.2413113612183</v>
+      </c>
       <c r="K10" s="3">
         <v>43705</v>
       </c>
       <c r="L10" s="5">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="M10" s="5">
         <v>958</v>
@@ -602,15 +695,25 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="E11" s="8">
+        <v>43708</v>
+      </c>
+      <c r="F11" s="7">
+        <v>-1586.979637395083</v>
+      </c>
+      <c r="G11" s="7">
+        <f>SUM($F$5:F11)+CurrentInventory</f>
+        <v>430.26167396613528</v>
+      </c>
       <c r="K11" s="3">
         <v>43705</v>
       </c>
       <c r="L11" s="5">
-        <v>12000</v>
+        <v>4000</v>
       </c>
       <c r="M11" s="5">
         <v>910</v>
@@ -619,13 +722,23 @@
         <v>1658</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="2">
         <v>0.45</v>
       </c>
+      <c r="E12" s="8">
+        <v>43709</v>
+      </c>
+      <c r="F12" s="7">
+        <v>-430.26167396613528</v>
+      </c>
+      <c r="G12" s="7">
+        <f>SUM($F$5:F12)+CurrentInventory</f>
+        <v>0</v>
+      </c>
       <c r="K12" s="3">
         <v>43709</v>
       </c>
@@ -639,13 +752,23 @@
         <v>1479.25</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="6">
         <v>5.0000000000000001E-4</v>
       </c>
+      <c r="E13" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F13" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G13" s="7" t="e">
+        <f>SUM($F$5:F13)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
       <c r="K13" s="3">
         <v>43709</v>
       </c>
@@ -659,7 +782,17 @@
         <v>1638.33</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E14" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F14" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G14" s="7" t="e">
+        <f>SUM($F$5:F14)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
       <c r="K14" s="3">
         <v>43709</v>
       </c>
@@ -673,13 +806,23 @@
         <v>1659.6699999999998</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="2">
         <v>500</v>
       </c>
+      <c r="E15" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F15" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G15" s="7" t="e">
+        <f>SUM($F$5:F15)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
       <c r="K15" s="3">
         <v>43709</v>
       </c>
@@ -693,103 +836,193 @@
         <v>1730.48</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E16" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F16" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G16" s="7" t="e">
+        <f>SUM($F$5:F16)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
       <c r="K16" s="3"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="2">
         <v>100</v>
+      </c>
+      <c r="E17" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F17" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G17" s="7" t="e">
+        <f>SUM($F$5:F17)+CurrentInventory</f>
+        <v>#N/A</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E18" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F18" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G18" s="7" t="e">
+        <f>SUM($F$5:F18)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
       <c r="K18" s="3"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="E19" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F19" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G19" s="7" t="e">
+        <f>SUM($F$5:F19)+CurrentInventory</f>
+        <v>#N/A</v>
       </c>
       <c r="K19" s="3"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="E20" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F20" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G20" s="7" t="e">
+        <f>SUM($F$5:F20)+CurrentInventory</f>
+        <v>#N/A</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>43702</v>
       </c>
       <c r="C21" s="4">
         <v>50.640695748227039</v>
+      </c>
+      <c r="E21" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F21" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G21" s="7" t="e">
+        <f>SUM($F$5:F21)+CurrentInventory</f>
+        <v>#N/A</v>
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f>B21+1</f>
         <v>43703</v>
       </c>
       <c r="C22" s="4">
         <v>49.700092287036142</v>
+      </c>
+      <c r="E22" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F22" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G22" s="7" t="e">
+        <f>SUM($F$5:F22)+CurrentInventory</f>
+        <v>#N/A</v>
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" ref="B23:B30" si="0">B22+1</f>
         <v>43704</v>
       </c>
       <c r="C23" s="4">
         <v>49.035222594048932</v>
+      </c>
+      <c r="E23" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F23" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G23" s="7" t="e">
+        <f>SUM($F$5:F23)+CurrentInventory</f>
+        <v>#N/A</v>
       </c>
       <c r="K23" s="3"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>43705</v>
       </c>
       <c r="C24" s="4">
         <v>49.257364798794171</v>
+      </c>
+      <c r="E24" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F24" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G24" s="7" t="e">
+        <f>SUM($F$5:F24)+CurrentInventory</f>
+        <v>#N/A</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>43706</v>
@@ -797,8 +1030,18 @@
       <c r="C25" s="4">
         <v>50.16228238269035</v>
       </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="E25" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F25" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G25" s="7" t="e">
+        <f>SUM($F$5:F25)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>43707</v>
@@ -806,8 +1049,18 @@
       <c r="C26" s="4">
         <v>50.917998292344571</v>
       </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="E26" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F26" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G26" s="7" t="e">
+        <f>SUM($F$5:F26)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>43708</v>
@@ -815,8 +1068,18 @@
       <c r="C27" s="4">
         <v>50.829710805583225</v>
       </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="E27" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F27" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G27" s="7" t="e">
+        <f>SUM($F$5:F27)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>43709</v>
@@ -824,8 +1087,18 @@
       <c r="C28" s="4">
         <v>49.978591030576084</v>
       </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="E28" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F28" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G28" s="7" t="e">
+        <f>SUM($F$5:F28)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>43710</v>
@@ -833,8 +1106,18 @@
       <c r="C29" s="4">
         <v>49.147154563324776</v>
       </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="E29" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F29" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G29" s="7" t="e">
+        <f>SUM($F$5:F29)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>43711</v>
@@ -842,272 +1125,832 @@
       <c r="C30" s="4">
         <v>49.099820257454425</v>
       </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="E30" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F30" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G30" s="7" t="e">
+        <f>SUM($F$5:F30)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
       <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="E31" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F31" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G31" s="7" t="e">
+        <f>SUM($F$5:F31)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
       <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E32" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F32" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G32" s="7" t="e">
+        <f>SUM($F$5:F32)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
       <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E33" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F33" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G33" s="7" t="e">
+        <f>SUM($F$5:F33)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E34" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F34" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G34" s="7" t="e">
+        <f>SUM($F$5:F34)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E35" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F35" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G35" s="7" t="e">
+        <f>SUM($F$5:F35)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
       <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E36" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F36" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G36" s="7" t="e">
+        <f>SUM($F$5:F36)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="3"/>
       <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E37" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F37" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G37" s="7" t="e">
+        <f>SUM($F$5:F37)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
       <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E38" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F38" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G38" s="7" t="e">
+        <f>SUM($F$5:F38)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
       <c r="C39" s="2"/>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E39" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F39" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G39" s="7" t="e">
+        <f>SUM($F$5:F39)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
       <c r="C40" s="2"/>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E40" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F40" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G40" s="7" t="e">
+        <f>SUM($F$5:F40)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
       <c r="C41" s="2"/>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E41" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F41" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G41" s="7" t="e">
+        <f>SUM($F$5:F41)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
       <c r="C42" s="2"/>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E42" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F42" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G42" s="7" t="e">
+        <f>SUM($F$5:F42)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
       <c r="C43" s="2"/>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E43" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F43" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G43" s="7" t="e">
+        <f>SUM($F$5:F43)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
       <c r="C44" s="2"/>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E44" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F44" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G44" s="7" t="e">
+        <f>SUM($F$5:F44)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="3"/>
       <c r="C45" s="2"/>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E45" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F45" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G45" s="7" t="e">
+        <f>SUM($F$5:F45)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="3"/>
       <c r="C46" s="2"/>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E46" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F46" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G46" s="7" t="e">
+        <f>SUM($F$5:F46)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="3"/>
       <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E47" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F47" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G47" s="7" t="e">
+        <f>SUM($F$5:F47)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="3"/>
       <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E48" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F48" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G48" s="7" t="e">
+        <f>SUM($F$5:F48)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="3"/>
       <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E49" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F49" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G49" s="7" t="e">
+        <f>SUM($F$5:F49)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="3"/>
       <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E50" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F50" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G50" s="7" t="e">
+        <f>SUM($F$5:F50)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" s="3"/>
       <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E51" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F51" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G51" s="7" t="e">
+        <f>SUM($F$5:F51)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" s="3"/>
       <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E52" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F52" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G52" s="7" t="e">
+        <f>SUM($F$5:F52)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="3"/>
       <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E53" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F53" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G53" s="7" t="e">
+        <f>SUM($F$5:F53)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
       <c r="C54" s="2"/>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E54" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F54" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G54" s="7" t="e">
+        <f>SUM($F$5:F54)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" s="3"/>
       <c r="C55" s="2"/>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E55" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F55" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G55" s="7" t="e">
+        <f>SUM($F$5:F55)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" s="3"/>
       <c r="C56" s="2"/>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E56" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F56" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G56" s="7" t="e">
+        <f>SUM($F$5:F56)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" s="3"/>
       <c r="C57" s="2"/>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E57" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F57" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G57" s="7" t="e">
+        <f>SUM($F$5:F57)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="3"/>
       <c r="C58" s="2"/>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E58" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F58" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G58" s="7" t="e">
+        <f>SUM($F$5:F58)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="3"/>
       <c r="C59" s="2"/>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E59" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F59" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G59" s="7" t="e">
+        <f>SUM($F$5:F59)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="3"/>
       <c r="C60" s="2"/>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E60" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F60" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G60" s="7" t="e">
+        <f>SUM($F$5:F60)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" s="3"/>
       <c r="C61" s="2"/>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E61" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F61" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G61" s="7" t="e">
+        <f>SUM($F$5:F61)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62" s="3"/>
       <c r="C62" s="2"/>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E62" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F62" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G62" s="7" t="e">
+        <f>SUM($F$5:F62)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63" s="3"/>
       <c r="C63" s="2"/>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E63" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F63" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G63" s="7" t="e">
+        <f>SUM($F$5:F63)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64" s="3"/>
       <c r="C64" s="2"/>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E64" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F64" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G64" s="7" t="e">
+        <f>SUM($F$5:F64)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" s="3"/>
       <c r="C65" s="2"/>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E65" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F65" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G65" s="7" t="e">
+        <f>SUM($F$5:F65)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="3"/>
       <c r="C66" s="2"/>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E66" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F66" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G66" s="7" t="e">
+        <f>SUM($F$5:F66)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="3"/>
       <c r="C67" s="2"/>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E67" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F67" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G67" s="7" t="e">
+        <f>SUM($F$5:F67)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" s="3"/>
       <c r="C68" s="2"/>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E68" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F68" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G68" s="7" t="e">
+        <f>SUM($F$5:F68)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" s="3"/>
       <c r="C69" s="2"/>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E69" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F69" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G69" s="7" t="e">
+        <f>SUM($F$5:F69)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" s="3"/>
       <c r="C70" s="2"/>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E70" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F70" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G70" s="7" t="e">
+        <f>SUM($F$5:F70)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" s="3"/>
       <c r="C71" s="2"/>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E71" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F71" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G71" s="7" t="e">
+        <f>SUM($F$5:F71)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" s="3"/>
       <c r="C72" s="2"/>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E72" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F72" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G72" s="7" t="e">
+        <f>SUM($F$5:F72)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" s="3"/>
       <c r="C73" s="2"/>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E73" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F73" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G73" s="7" t="e">
+        <f>SUM($F$5:F73)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" s="3"/>
       <c r="C74" s="2"/>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E74" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F74" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G74" s="7" t="e">
+        <f>SUM($F$5:F74)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" s="3"/>
       <c r="C75" s="2"/>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E75" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F75" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G75" s="7" t="e">
+        <f>SUM($F$5:F75)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76" s="3"/>
       <c r="C76" s="2"/>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E76" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F76" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G76" s="7" t="e">
+        <f>SUM($F$5:F76)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77" s="3"/>
       <c r="C77" s="2"/>
-    </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E77" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F77" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G77" s="7" t="e">
+        <f>SUM($F$5:F77)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78" s="3"/>
       <c r="C78" s="2"/>
-    </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E78" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F78" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G78" s="7" t="e">
+        <f>SUM($F$5:F78)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79" s="3"/>
       <c r="C79" s="2"/>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E79" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F79" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G79" s="7" t="e">
+        <f>SUM($F$5:F79)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" s="3"/>
       <c r="C80" s="2"/>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E80" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F80" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G80" s="7" t="e">
+        <f>SUM($F$5:F80)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" s="3"/>
       <c r="C81" s="2"/>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E81" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F81" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G81" s="7" t="e">
+        <f>SUM($F$5:F81)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" s="3"/>
       <c r="C82" s="2"/>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E82" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F82" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G82" s="7" t="e">
+        <f>SUM($F$5:F82)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="3"/>
       <c r="C83" s="2"/>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E83" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F83" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G83" s="7" t="e">
+        <f>SUM($F$5:F83)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" s="3"/>
       <c r="C84" s="2"/>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E84" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F84" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G84" s="7" t="e">
+        <f>SUM($F$5:F84)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="3"/>
       <c r="C85" s="2"/>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="E85" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F85" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G85" s="7" t="e">
+        <f>SUM($F$5:F85)+CurrentInventory</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" s="3"/>
       <c r="C86" s="2"/>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" s="3"/>
       <c r="C87" s="2"/>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" s="3"/>
       <c r="C88" s="2"/>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="3"/>
       <c r="C89" s="2"/>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="3"/>
       <c r="C90" s="2"/>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" s="3"/>
       <c r="C91" s="2"/>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" s="3"/>
       <c r="C92" s="2"/>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93" s="3"/>
       <c r="C93" s="2"/>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" s="3"/>
       <c r="C94" s="2"/>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" s="3"/>
       <c r="C95" s="2"/>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" s="3"/>
       <c r="C96" s="2"/>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" s="3"/>
       <c r="C97" s="2"/>
     </row>

</xml_diff>

<commit_message>
Added Excel function which returns the add-in version.
</commit_message>
<xml_diff>
--- a/samples/excel/storage_samples.xlsx
+++ b/samples/excel/storage_samples.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D133F8CE-C3A1-4C9D-AE8B-0DD6C7A924A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1F5B85-BF0F-4967-9C4E-9B8B03892188}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="intrinsic_daily" sheetId="1" r:id="rId1"/>
+    <sheet name="info" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="CurrentInventory">intrinsic_daily!$C$15</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Valuation Date</t>
   </si>
@@ -95,13 +96,16 @@
   <si>
     <t>Inject/Withdraw</t>
   </si>
+  <si>
+    <t>Storage Add-in Version</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="164" formatCode="dd\-mmm\-yy"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -166,7 +170,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -175,7 +179,8 @@
     <xf numFmtId="4" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -460,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1958,4 +1963,32 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636FAECC-9A00-42A4-9A91-44F0AC0942A7}">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="9" t="str">
+        <f>_xll.cmdty.StorageAddInVersion()</f>
+        <v>0.1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated dna file with renamed dll: Cmdty.Storage.Core.dll -> Cmdty.Storage.dll
</commit_message>
<xml_diff>
--- a/samples/excel/storage_samples.xlsx
+++ b/samples/excel/storage_samples.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1F5B85-BF0F-4967-9C4E-9B8B03892188}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCA4E19-1482-4388-A685-097084C1ECF7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="intrinsic_daily" sheetId="1" r:id="rId1"/>
@@ -465,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
       </c>
       <c r="F1" s="7">
         <f>_xll.cmdty.StorageIntrinsicValue(ValDate,StorageStart,StorageEnd,K5:N24,InjectCostRate,InjectCmdtyConsumed,WithdrawCostRate,WithdrawCmdtyConsumed,CurrentInventory,B21:C97,,GridSpacing)</f>
-        <v>28160.178279742478</v>
+        <v>28157.587119216052</v>
       </c>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
@@ -862,7 +862,8 @@
         <v>1</v>
       </c>
       <c r="C17" s="2">
-        <v>100</v>
+        <f>MAX(L5:L24)/100</f>
+        <v>120</v>
       </c>
       <c r="E17" s="8" t="e">
         <v>#N/A</v>
@@ -1969,7 +1970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636FAECC-9A00-42A4-9A91-44F0AC0942A7}">
   <dimension ref="B2:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Made numerical tolerance a parameter to calculation of bang-bang decision set.
</commit_message>
<xml_diff>
--- a/samples/excel/storage_samples.xlsx
+++ b/samples/excel/storage_samples.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DF7510-C048-4C9E-A119-C46CF9AA378A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F361F0-C90F-4915-B150-CC52FC95785A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -521,7 +521,7 @@
   <dimension ref="B2:P1596"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +594,7 @@
         <v>15</v>
       </c>
       <c r="O4" s="7">
-        <f t="array" ref="O4">_xll.cmdty.StorageIntrinsicValue(ValDate,StorageStart,StorageEnd,I5:L290,InjectCostRate,InjectCmdtyConsumed,WithdrawCostRate,WithdrawCmdtyConsumed,CurrentInventory,E21:F1596,,GridSpacing)</f>
+        <f>_xll.cmdty.StorageIntrinsicValue(ValDate,StorageStart,StorageEnd,I5:L290,InjectCostRate,InjectCmdtyConsumed,WithdrawCostRate,WithdrawCmdtyConsumed,CurrentInventory,E21:F1596,,GridSpacing)</f>
         <v>293247.11229444161</v>
       </c>
     </row>

</xml_diff>